<commit_message>
feat: integrate Belgian architect fee calculator and update related logic in expense calculations
</commit_message>
<xml_diff>
--- a/apps/web/test_xlsx_output.xlsx
+++ b/apps/web/test_xlsx_output.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z71"/>
+  <dimension ref="A1:Z75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -627,573 +627,611 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>HONORAIRES (15% × 30% CASCO hors TVA sur 3 ans)</v>
+        <v>HONORAIRES ARCHITECTE (formule belge)</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v xml:space="preserve">  Base CASCO hors TVA</v>
+        <v xml:space="preserve">  Surface totale</v>
       </c>
       <c r="B30">
-        <v>760040</v>
+        <v>246</v>
+      </c>
+      <c r="C30" t="str">
+        <v>m²</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v xml:space="preserve">  Honoraires par an</v>
+        <v xml:space="preserve">  Coût CASCO hors TVA</v>
       </c>
       <c r="B31">
-        <v>11400.599999999999</v>
+        <v>760040</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v xml:space="preserve">  Honoraires total 3 ans</v>
-      </c>
-      <c r="B32">
-        <v>34201.799999999996</v>
+        <v xml:space="preserve">  Type projet</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Immeuble à appartements</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>FRAIS RECURRENTS (3 ans)</v>
+        <v xml:space="preserve">  Type bâtiment</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Rénovation</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v xml:space="preserve">  Précompte immobilier</v>
+        <v xml:space="preserve">  Heures estimées</v>
       </c>
       <c r="B34">
-        <v>388.38</v>
+        <v>708</v>
       </c>
       <c r="C34" t="str">
-        <v>388.38/an × 3 ans</v>
+        <v>h × 60 €/h</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v xml:space="preserve">  Comptable</v>
+        <v xml:space="preserve">  Honoraires par an</v>
       </c>
       <c r="B35">
-        <v>1000</v>
-      </c>
-      <c r="C35" t="str">
-        <v>1000/an × 3 ans</v>
+        <v>14170</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v xml:space="preserve">  Podio abonnement</v>
+        <v xml:space="preserve">  Honoraires total</v>
       </c>
       <c r="B36">
-        <v>600</v>
-      </c>
-      <c r="C36" t="str">
-        <v>600/an × 3 ans</v>
+        <v>42510</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v xml:space="preserve">  Assurance bâtiment</v>
-      </c>
-      <c r="B37">
-        <v>2000</v>
-      </c>
-      <c r="C37" t="str">
-        <v>2000/an × 3 ans</v>
+        <v>FRAIS RECURRENTS (3 ans)</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v xml:space="preserve">  Frais réservation</v>
+        <v xml:space="preserve">  Précompte immobilier</v>
       </c>
       <c r="B38">
-        <v>2000</v>
+        <v>388.38</v>
       </c>
       <c r="C38" t="str">
-        <v>2000/an × 3 ans</v>
+        <v>388.38/an × 3 ans</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v xml:space="preserve">  Imprévus</v>
+        <v xml:space="preserve">  Comptable</v>
       </c>
       <c r="B39">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C39" t="str">
-        <v>2000/an × 3 ans</v>
+        <v>1000/an × 3 ans</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v xml:space="preserve">  Total récurrents 3 ans</v>
+        <v xml:space="preserve">  Podio abonnement</v>
       </c>
       <c r="B40">
-        <v>23965.14</v>
+        <v>600</v>
+      </c>
+      <c r="C40" t="str">
+        <v>600/an × 3 ans</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>FRAIS PONCTUELS</v>
+        <v xml:space="preserve">  Assurance bâtiment</v>
+      </c>
+      <c r="B41">
+        <v>2000</v>
+      </c>
+      <c r="C41" t="str">
+        <v>2000/an × 3 ans</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v xml:space="preserve">  Frais dossier crédit</v>
+        <v xml:space="preserve">  Frais réservation</v>
       </c>
       <c r="B42">
-        <v>500</v>
+        <v>2000</v>
+      </c>
+      <c r="C42" t="str">
+        <v>2000/an × 3 ans</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v xml:space="preserve">  Frais gestion crédit</v>
+        <v xml:space="preserve">  Imprévus</v>
       </c>
       <c r="B43">
-        <v>45</v>
+        <v>2000</v>
+      </c>
+      <c r="C43" t="str">
+        <v>2000/an × 3 ans</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v xml:space="preserve">  Frais notaire base partagée</v>
+        <v xml:space="preserve">  Total récurrents 3 ans</v>
       </c>
       <c r="B44">
-        <v>5000</v>
+        <v>23965.14</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v xml:space="preserve">  Total ponctuels</v>
-      </c>
-      <c r="B45">
-        <v>5545</v>
+        <v>FRAIS PONCTUELS</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>TOTAL FRAIS GENERAUX</v>
+        <v xml:space="preserve">  Frais dossier crédit</v>
       </c>
       <c r="B46">
-        <v>63711.939999999995</v>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v xml:space="preserve">  Frais gestion crédit</v>
+      </c>
+      <c r="B47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v xml:space="preserve">  Frais notaire base partagée</v>
+      </c>
+      <c r="B48">
+        <v>5000</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>DETAILS PAR TYPE D UNITE</v>
+        <v xml:space="preserve">  Total ponctuels</v>
+      </c>
+      <c r="B49">
+        <v>5545</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>Unite 1</v>
-      </c>
-      <c r="B50" t="str">
-        <v>CASCO: 178080, Parachèvements: 56000</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="str">
-        <v>Unite 3</v>
-      </c>
-      <c r="B51" t="str">
-        <v>CASCO: 213060, Parachèvements: 67000</v>
+        <v>TOTAL FRAIS GENERAUX</v>
+      </c>
+      <c r="B50">
+        <v>72020.14</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>DETAILS PAR TYPE D UNITE</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>DECOMPOSITION DES COUTS</v>
+        <v>Unite 1</v>
+      </c>
+      <c r="B54" t="str">
+        <v>CASCO: 178080, Parachèvements: 56000</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>Achat Total</v>
-      </c>
-      <c r="B55">
-        <f>B5</f>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="str">
-        <v>Droit enreg. + Frais notaire</v>
-      </c>
-      <c r="B56">
-        <f>SUM(J60:K61)</f>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="str">
-        <v>Construction</v>
-      </c>
-      <c r="B57">
-        <f>SUM(O60:O61)</f>
+        <v>Unite 3</v>
+      </c>
+      <c r="B55" t="str">
+        <v>CASCO: 213060, Parachèvements: 67000</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>Commun Infrastructure</v>
-      </c>
-      <c r="B58">
-        <f>B18</f>
+        <v>DECOMPOSITION DES COUTS</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>Nom</v>
-      </c>
-      <c r="B59" t="str">
-        <v>Unite</v>
-      </c>
-      <c r="C59" t="str">
-        <v>Surface</v>
-      </c>
-      <c r="D59" t="str">
-        <v>Qty</v>
-      </c>
-      <c r="E59" t="str">
-        <v>Capital</v>
-      </c>
-      <c r="F59" t="str">
-        <v>Taux notaire</v>
-      </c>
-      <c r="G59" t="str">
-        <v>Taux interet</v>
-      </c>
-      <c r="H59" t="str">
-        <v>Duree (ans)</v>
-      </c>
-      <c r="I59" t="str">
-        <v>Part achat</v>
-      </c>
-      <c r="J59" t="str">
-        <v>Droit enreg.</v>
-      </c>
-      <c r="K59" t="str">
-        <v>Frais notaire</v>
-      </c>
-      <c r="L59" t="str">
-        <v>CASCO</v>
-      </c>
-      <c r="M59" t="str">
-        <v>Parachevements</v>
-      </c>
-      <c r="N59" t="str">
-        <v>Travaux communs</v>
-      </c>
-      <c r="O59" t="str">
-        <v>Construction</v>
-      </c>
-      <c r="P59" t="str">
-        <v>Commun</v>
-      </c>
-      <c r="Q59" t="str">
-        <v>TOTAL</v>
-      </c>
-      <c r="R59" t="str">
-        <v>Emprunt</v>
-      </c>
-      <c r="S59" t="str">
-        <v>Mensualite</v>
-      </c>
-      <c r="T59" t="str">
-        <v>Total rembourse</v>
-      </c>
-      <c r="U59" t="str">
-        <v>Reno perso</v>
-      </c>
-      <c r="V59" t="str">
-        <v>CASCO m2</v>
-      </c>
-      <c r="W59" t="str">
-        <v>Parachev m2</v>
-      </c>
-      <c r="X59" t="str">
-        <v>CASCO sqm</v>
-      </c>
-      <c r="Y59" t="str">
-        <v>Parachev sqm</v>
-      </c>
-      <c r="Z59" t="str">
-        <v>Fondateur</v>
+        <v>Achat Total</v>
+      </c>
+      <c r="B59">
+        <f>B5</f>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>Manuela/Dragan</v>
+        <v>Droit enreg. + Frais notaire</v>
       </c>
       <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60">
-        <v>112</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60">
-        <v>50000</v>
-      </c>
-      <c r="F60">
-        <v>12.5</v>
-      </c>
-      <c r="G60">
-        <v>4.5</v>
-      </c>
-      <c r="H60">
-        <v>25</v>
-      </c>
-      <c r="I60">
-        <f>C60*$B$7</f>
-      </c>
-      <c r="J60">
-        <f>I60*F60/100</f>
-      </c>
-      <c r="K60">
-        <f>D60*1000</f>
-      </c>
-      <c r="L60">
-        <v>178080</v>
-      </c>
-      <c r="M60">
-        <v>56000</v>
-      </c>
-      <c r="N60">
-        <f>$B$26</f>
-      </c>
-      <c r="O60">
-        <f>(L60+M60)+N60*D60</f>
-      </c>
-      <c r="P60">
-        <f>$B$19</f>
-      </c>
-      <c r="Q60">
-        <f>I60+J60+K60+O60+P60</f>
-      </c>
-      <c r="R60">
-        <f>Q60-E60</f>
-      </c>
-      <c r="S60">
-        <f>PMT(G60/100/12,H60*12,R60)*-1</f>
-      </c>
-      <c r="T60">
-        <f>S60*H60*12</f>
-      </c>
-      <c r="U60">
-        <v>234080</v>
-      </c>
-      <c r="V60">
-        <v>1590</v>
-      </c>
-      <c r="Z60" t="str">
-        <v>Non</v>
+        <f>SUM(J64:K65)</f>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>Cathy/Jim</v>
+        <v>Construction</v>
       </c>
       <c r="B61">
-        <v>3</v>
-      </c>
-      <c r="C61">
-        <v>134</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61">
-        <v>170000</v>
-      </c>
-      <c r="F61">
-        <v>12.5</v>
-      </c>
-      <c r="G61">
-        <v>4.5</v>
-      </c>
-      <c r="H61">
-        <v>25</v>
-      </c>
-      <c r="I61">
-        <f>C61*$B$7</f>
-      </c>
-      <c r="J61">
-        <f>I61*F61/100</f>
-      </c>
-      <c r="K61">
-        <f>D61*1000</f>
-      </c>
-      <c r="L61">
-        <v>213060</v>
-      </c>
-      <c r="M61">
-        <v>67000</v>
-      </c>
-      <c r="N61">
-        <f>$B$26</f>
-      </c>
-      <c r="O61">
-        <f>(L61+M61)+N61*D61</f>
-      </c>
-      <c r="P61">
-        <f>$B$19</f>
-      </c>
-      <c r="Q61">
-        <f>I61+J61+K61+O61+P61</f>
-      </c>
-      <c r="R61">
-        <f>Q61-E61</f>
-      </c>
-      <c r="S61">
-        <f>PMT(G61/100/12,H61*12,R61)*-1</f>
-      </c>
-      <c r="T61">
-        <f>S61*H61*12</f>
-      </c>
-      <c r="U61">
-        <v>280060</v>
-      </c>
-      <c r="V61">
-        <v>1590</v>
-      </c>
-      <c r="Z61" t="str">
-        <v>Non</v>
+        <f>SUM(O64:O65)</f>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
+        <v>Commun Infrastructure</v>
+      </c>
+      <c r="B62">
+        <f>B18</f>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Nom</v>
+      </c>
+      <c r="B63" t="str">
+        <v>Unite</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Surface</v>
+      </c>
+      <c r="D63" t="str">
+        <v>Qty</v>
+      </c>
+      <c r="E63" t="str">
+        <v>Capital</v>
+      </c>
+      <c r="F63" t="str">
+        <v>Taux notaire</v>
+      </c>
+      <c r="G63" t="str">
+        <v>Taux interet</v>
+      </c>
+      <c r="H63" t="str">
+        <v>Duree (ans)</v>
+      </c>
+      <c r="I63" t="str">
+        <v>Part achat</v>
+      </c>
+      <c r="J63" t="str">
+        <v>Droit enreg.</v>
+      </c>
+      <c r="K63" t="str">
+        <v>Frais notaire</v>
+      </c>
+      <c r="L63" t="str">
+        <v>CASCO</v>
+      </c>
+      <c r="M63" t="str">
+        <v>Parachevements</v>
+      </c>
+      <c r="N63" t="str">
+        <v>Travaux communs</v>
+      </c>
+      <c r="O63" t="str">
+        <v>Construction</v>
+      </c>
+      <c r="P63" t="str">
+        <v>Commun</v>
+      </c>
+      <c r="Q63" t="str">
         <v>TOTAL</v>
       </c>
-      <c r="B62" t="str">
-        <v/>
-      </c>
-      <c r="C62">
-        <f>SUM(C60:C61)</f>
-      </c>
-      <c r="D62">
-        <f>SUM(D60:D61)</f>
-      </c>
-      <c r="E62">
-        <f>SUM(E60:E61)</f>
-      </c>
-      <c r="F62" t="str">
-        <v/>
-      </c>
-      <c r="G62" t="str">
-        <v/>
-      </c>
-      <c r="H62" t="str">
-        <v/>
-      </c>
-      <c r="I62">
-        <f>SUM(I60:I61)</f>
-      </c>
-      <c r="J62">
-        <f>SUM(J60:J61)</f>
-      </c>
-      <c r="K62">
-        <f>SUM(K60:K61)</f>
-      </c>
-      <c r="L62">
-        <f>SUM(L60:L61)</f>
-      </c>
-      <c r="M62">
-        <f>SUM(M60:M61)</f>
-      </c>
-      <c r="N62">
-        <f>SUM(N60:N61)</f>
-      </c>
-      <c r="O62">
-        <f>SUM(O60:O61)</f>
-      </c>
-      <c r="P62">
-        <f>SUM(P60:P61)</f>
-      </c>
-      <c r="Q62">
-        <f>SUM(Q60:Q61)</f>
-      </c>
-      <c r="R62" t="str">
-        <v/>
-      </c>
-      <c r="S62">
-        <f>SUM(S60:S61)</f>
-      </c>
-      <c r="T62">
-        <f>SUM(T60:T61)</f>
-      </c>
-      <c r="U62" t="str">
-        <v/>
-      </c>
-      <c r="V62" t="str">
-        <v/>
-      </c>
-      <c r="W62" t="str">
-        <v/>
-      </c>
-      <c r="X62" t="str">
-        <v/>
-      </c>
-      <c r="Y62" t="str">
-        <v/>
-      </c>
-      <c r="Z62" t="str">
-        <v/>
+      <c r="R63" t="str">
+        <v>Emprunt</v>
+      </c>
+      <c r="S63" t="str">
+        <v>Mensualite</v>
+      </c>
+      <c r="T63" t="str">
+        <v>Total rembourse</v>
+      </c>
+      <c r="U63" t="str">
+        <v>Reno perso</v>
+      </c>
+      <c r="V63" t="str">
+        <v>CASCO m2</v>
+      </c>
+      <c r="W63" t="str">
+        <v>Parachev m2</v>
+      </c>
+      <c r="X63" t="str">
+        <v>CASCO sqm</v>
+      </c>
+      <c r="Y63" t="str">
+        <v>Parachev sqm</v>
+      </c>
+      <c r="Z63" t="str">
+        <v>Fondateur</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Manuela/Dragan</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>112</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>50000</v>
+      </c>
+      <c r="F64">
+        <v>12.5</v>
+      </c>
+      <c r="G64">
+        <v>4.5</v>
+      </c>
+      <c r="H64">
+        <v>25</v>
+      </c>
+      <c r="I64">
+        <f>C64*$B$7</f>
+      </c>
+      <c r="J64">
+        <f>I64*F64/100</f>
+      </c>
+      <c r="K64">
+        <f>D64*1000</f>
+      </c>
+      <c r="L64">
+        <v>178080</v>
+      </c>
+      <c r="M64">
+        <v>56000</v>
+      </c>
+      <c r="N64">
+        <f>$B$26</f>
+      </c>
+      <c r="O64">
+        <f>(L64+M64)+N64*D64</f>
+      </c>
+      <c r="P64">
+        <f>$B$19</f>
+      </c>
+      <c r="Q64">
+        <f>I64+J64+K64+O64+P64</f>
+      </c>
+      <c r="R64">
+        <f>Q64-E64</f>
+      </c>
+      <c r="S64">
+        <f>PMT(G64/100/12,H64*12,R64)*-1</f>
+      </c>
+      <c r="T64">
+        <f>S64*H64*12</f>
+      </c>
+      <c r="U64">
+        <v>234080</v>
+      </c>
+      <c r="V64">
+        <v>1590</v>
+      </c>
+      <c r="Z64" t="str">
+        <v>Non</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>SYNTHESE GLOBALE</v>
+        <v>Cathy/Jim</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <v>134</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>170000</v>
+      </c>
+      <c r="F65">
+        <v>12.5</v>
+      </c>
+      <c r="G65">
+        <v>4.5</v>
+      </c>
+      <c r="H65">
+        <v>25</v>
+      </c>
+      <c r="I65">
+        <f>C65*$B$7</f>
+      </c>
+      <c r="J65">
+        <f>I65*F65/100</f>
+      </c>
+      <c r="K65">
+        <f>D65*1000</f>
+      </c>
+      <c r="L65">
+        <v>213060</v>
+      </c>
+      <c r="M65">
+        <v>67000</v>
+      </c>
+      <c r="N65">
+        <f>$B$26</f>
+      </c>
+      <c r="O65">
+        <f>(L65+M65)+N65*D65</f>
+      </c>
+      <c r="P65">
+        <f>$B$19</f>
+      </c>
+      <c r="Q65">
+        <f>I65+J65+K65+O65+P65</f>
+      </c>
+      <c r="R65">
+        <f>Q65-E65</f>
+      </c>
+      <c r="S65">
+        <f>PMT(G65/100/12,H65*12,R65)*-1</f>
+      </c>
+      <c r="T65">
+        <f>S65*H65*12</f>
+      </c>
+      <c r="U65">
+        <v>280060</v>
+      </c>
+      <c r="V65">
+        <v>1590</v>
+      </c>
+      <c r="Z65" t="str">
+        <v>Non</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>Cout total projet</v>
-      </c>
-      <c r="B66">
-        <f>P62</f>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="str">
-        <v>Capital total apporte</v>
-      </c>
-      <c r="B67">
-        <f>E62</f>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="str">
-        <v>Total emprunts necessaires</v>
-      </c>
-      <c r="B68">
-        <f>Q62</f>
+        <v>TOTAL</v>
+      </c>
+      <c r="B66" t="str">
+        <v/>
+      </c>
+      <c r="C66">
+        <f>SUM(C64:C65)</f>
+      </c>
+      <c r="D66">
+        <f>SUM(D64:D65)</f>
+      </c>
+      <c r="E66">
+        <f>SUM(E64:E65)</f>
+      </c>
+      <c r="F66" t="str">
+        <v/>
+      </c>
+      <c r="G66" t="str">
+        <v/>
+      </c>
+      <c r="H66" t="str">
+        <v/>
+      </c>
+      <c r="I66">
+        <f>SUM(I64:I65)</f>
+      </c>
+      <c r="J66">
+        <f>SUM(J64:J65)</f>
+      </c>
+      <c r="K66">
+        <f>SUM(K64:K65)</f>
+      </c>
+      <c r="L66">
+        <f>SUM(L64:L65)</f>
+      </c>
+      <c r="M66">
+        <f>SUM(M64:M65)</f>
+      </c>
+      <c r="N66">
+        <f>SUM(N64:N65)</f>
+      </c>
+      <c r="O66">
+        <f>SUM(O64:O65)</f>
+      </c>
+      <c r="P66">
+        <f>SUM(P64:P65)</f>
+      </c>
+      <c r="Q66">
+        <f>SUM(Q64:Q65)</f>
+      </c>
+      <c r="R66" t="str">
+        <v/>
+      </c>
+      <c r="S66">
+        <f>SUM(S64:S65)</f>
+      </c>
+      <c r="T66">
+        <f>SUM(T64:T65)</f>
+      </c>
+      <c r="U66" t="str">
+        <v/>
+      </c>
+      <c r="V66" t="str">
+        <v/>
+      </c>
+      <c r="W66" t="str">
+        <v/>
+      </c>
+      <c r="X66" t="str">
+        <v/>
+      </c>
+      <c r="Y66" t="str">
+        <v/>
+      </c>
+      <c r="Z66" t="str">
+        <v/>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>Emprunt moyen</v>
-      </c>
-      <c r="B69">
-        <f>AVERAGE(Q60:Q61)</f>
+        <v>SYNTHESE GLOBALE</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>Emprunt minimum</v>
+        <v>Cout total projet</v>
       </c>
       <c r="B70">
-        <f>MIN(Q60:Q61)</f>
+        <f>P66</f>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
+        <v>Capital total apporte</v>
+      </c>
+      <c r="B71">
+        <f>E66</f>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Total emprunts necessaires</v>
+      </c>
+      <c r="B72">
+        <f>Q66</f>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Emprunt moyen</v>
+      </c>
+      <c r="B73">
+        <f>AVERAGE(Q64:Q65)</f>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Emprunt minimum</v>
+      </c>
+      <c r="B74">
+        <f>MIN(Q64:Q65)</f>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
         <v>Emprunt maximum</v>
       </c>
-      <c r="B71">
-        <f>MAX(Q60:Q61)</f>
+      <c r="B75">
+        <f>MAX(Q64:Q65)</f>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Z71"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Z75"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>